<commit_message>
try again for rachel
</commit_message>
<xml_diff>
--- a/01.19.2024/financial_anal_template.xlsx
+++ b/01.19.2024/financial_anal_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ftfy repo\ftfy github repo\financialaudit\01.19.2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FFF03EC-CB8E-4BE5-8BAD-D2F82569970E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C1916-8572-4083-B8EF-1C4D911539A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EABEB508-9CDB-4E9C-9838-5B5F93A0A586}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{EABEB508-9CDB-4E9C-9838-5B5F93A0A586}"/>
   </bookViews>
   <sheets>
     <sheet name="General Template" sheetId="1" r:id="rId1"/>
@@ -776,7 +776,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -794,9 +794,6 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1171,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DAD69-0CBD-442A-B9B3-7BA41531C407}">
   <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,7 +1223,7 @@
       <c r="B7" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="12" t="s">
         <v>123</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -1243,7 +1240,7 @@
       <c r="B8" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
         <v>129</v>
       </c>
@@ -1289,7 +1286,7 @@
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1583,7 +1580,7 @@
       <c r="C60" t="s">
         <v>97</v>
       </c>
-      <c r="D60" s="20">
+      <c r="D60" s="17">
         <f>'Misc Expenses'!A1</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Video break at 15.31
</commit_message>
<xml_diff>
--- a/01.19.2024/financial_anal_template.xlsx
+++ b/01.19.2024/financial_anal_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\ftfy repo\ftfy github repo\financialaudit\01.19.2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C1916-8572-4083-B8EF-1C4D911539A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3155DFAF-4913-42EA-9B14-6F697EDDC6D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{EABEB508-9CDB-4E9C-9838-5B5F93A0A586}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Red Flags" sheetId="3" r:id="rId3"/>
     <sheet name="In This Economy" sheetId="4" r:id="rId4"/>
     <sheet name="Credit Score" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -115,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="167">
   <si>
     <t>Assets</t>
   </si>
@@ -189,9 +190,6 @@
     <t>Cash and Cash Equivalents</t>
   </si>
   <si>
-    <t>Wallet/Under the Mattress</t>
-  </si>
-  <si>
     <t>Savings Account</t>
   </si>
   <si>
@@ -588,9 +586,6 @@
     <t>Tax codes favor avoidance for those who own assets, not your avg Joe</t>
   </si>
   <si>
-    <t>Fidelity</t>
-  </si>
-  <si>
     <t>Brokerage/Stocks #3</t>
   </si>
   <si>
@@ -601,6 +596,27 @@
   </si>
   <si>
     <t>Under the Table</t>
+  </si>
+  <si>
+    <t>Rachel</t>
+  </si>
+  <si>
+    <t>Spiritual Coach</t>
+  </si>
+  <si>
+    <t>Penny Wise, Pound Foolish</t>
+  </si>
+  <si>
+    <t>withdrawing large amount</t>
+  </si>
+  <si>
+    <t>Acorn/Using as Checking, Withdrew all funds</t>
+  </si>
+  <si>
+    <t>Wallet/Cash Under the Mattress</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -776,7 +792,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -795,6 +811,7 @@
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1168,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DAD69-0CBD-442A-B9B3-7BA41531C407}">
   <dimension ref="A1:F133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,22 +1200,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D1" s="16" t="str">
         <f>IF(D65&lt;0,0,IF(AND(D65&gt;20000,D123&gt;1000000),10,"DEPENDS"))</f>
         <v>DEPENDS</v>
       </c>
       <c r="E1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -1210,43 +1227,49 @@
       <c r="A5" t="s">
         <v>9</v>
       </c>
+      <c r="B5" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
+      <c r="B6">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>125</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" s="13" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -1258,6 +1281,9 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -1276,7 +1302,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1286,7 +1312,7 @@
       <c r="B15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="18" t="s">
         <v>16</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -1301,16 +1327,16 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
         <v>26</v>
       </c>
-      <c r="E17" t="s">
-        <v>27</v>
-      </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1318,69 +1344,74 @@
         <v>3</v>
       </c>
       <c r="D18" s="6"/>
+      <c r="E18" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
         <f>SUM(D19:D27)</f>
-        <v>0</v>
+        <v>6500</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>141</v>
-      </c>
-      <c r="D21" s="7"/>
+      <c r="C21" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" s="7">
+        <v>6500</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D26" s="7"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D27" s="7"/>
       <c r="E27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1395,209 +1426,220 @@
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="15">
         <f>SUM(D30:D62)</f>
-        <v>0</v>
+        <v>5263.24</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="D30" s="8">
+        <v>2100</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D33" s="8"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D34" s="8"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C35" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C39" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D39" s="8"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C40" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D40" s="8"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C41" t="s">
-        <v>73</v>
-      </c>
-      <c r="D41" s="8"/>
+        <v>72</v>
+      </c>
+      <c r="D41" s="8">
+        <v>534</v>
+      </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D46" s="8"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C47" t="s">
-        <v>101</v>
-      </c>
-      <c r="D47" s="8"/>
+        <v>100</v>
+      </c>
+      <c r="D47" s="8">
+        <v>12</v>
+      </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48" s="8"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" s="8"/>
+        <v>78</v>
+      </c>
+      <c r="D49" s="8">
+        <v>99.49</v>
+      </c>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C53" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C54" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C55" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D55" s="8"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C57" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C59" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C60" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D60" s="17">
         <f>'Misc Expenses'!A1</f>
-        <v>0</v>
+        <v>1087.75</v>
       </c>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D61" s="8"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C62" t="s">
-        <v>107</v>
-      </c>
-      <c r="D62" s="8"/>
+        <v>106</v>
+      </c>
+      <c r="D62" s="8">
+        <f>0.22*D21</f>
+        <v>1430</v>
+      </c>
       <c r="E62" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
@@ -1608,37 +1650,37 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D65" s="5">
         <f>SUM(D19:D27)-SUM(D30:D62)</f>
-        <v>0</v>
+        <v>1236.7600000000002</v>
       </c>
       <c r="E65" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D66" s="5">
         <f>D65*12</f>
-        <v>0</v>
+        <v>14841.120000000003</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D69" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E69" t="s">
         <v>26</v>
       </c>
-      <c r="E69" t="s">
-        <v>27</v>
-      </c>
       <c r="F69" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
@@ -1655,34 +1697,43 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C72" t="s">
-        <v>24</v>
-      </c>
-      <c r="D72" s="9"/>
+        <v>165</v>
+      </c>
+      <c r="D72" s="9">
+        <v>600</v>
+      </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C73" t="s">
         <v>22</v>
       </c>
-      <c r="D73" s="9"/>
+      <c r="D73" s="9">
+        <v>4000</v>
+      </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C74" t="s">
-        <v>25</v>
-      </c>
-      <c r="D74" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="D74" s="9">
+        <v>100</v>
+      </c>
+      <c r="E74" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C75" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D75" s="9"/>
       <c r="F75" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C76" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D76" s="9"/>
     </row>
@@ -1694,136 +1745,138 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C78" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C79" t="s">
-        <v>145</v>
-      </c>
-      <c r="D79" s="9"/>
+        <v>144</v>
+      </c>
+      <c r="D79" s="9">
+        <v>0</v>
+      </c>
       <c r="E79" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C80" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C81" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D81" s="9"/>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C82" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D82" s="9"/>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C83" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D83" s="9"/>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C84" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D84" s="9"/>
       <c r="F84" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D85" s="9"/>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D86" s="9"/>
       <c r="F86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C87" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D87" s="9"/>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C89" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D89" s="9"/>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D90" s="9"/>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D91" s="9"/>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C92" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D92" s="9"/>
       <c r="E92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C93" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C94" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D95" s="9"/>
     </row>
@@ -1841,148 +1894,148 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D99" s="10"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C100" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D100" s="10"/>
       <c r="F100" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C101" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D101" s="10"/>
       <c r="F101" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C102" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D102" s="10"/>
       <c r="F102" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C103" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D103" s="10"/>
       <c r="F103" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D104" s="10"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C105" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D105" s="10"/>
       <c r="F105" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C106" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D106" s="10"/>
       <c r="F106" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D107" s="10"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C108" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D108" s="10"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D109" s="10"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C110" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D110" s="10"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C111" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D111" s="10"/>
       <c r="E111" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D112" s="10"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C113" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D113" s="10"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C114" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D114" s="10"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C115" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D115" s="10"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D116" s="10"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C117" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D117" s="10"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D118" s="10"/>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C119" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D119" s="10"/>
     </row>
@@ -1997,20 +2050,20 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D122" s="5"/>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C123" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D123" s="5">
         <f>SUM(D71:D96)-SUM(D99:D119)</f>
-        <v>0</v>
+        <v>4700</v>
       </c>
       <c r="E123" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -2021,22 +2074,22 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
@@ -2059,10 +2112,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48F88B4-CBA5-48C5-A530-FBAA80738C5A}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A13"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2073,15 +2126,15 @@
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="11">
         <f>SUM(A3:A40)</f>
-        <v>0</v>
+        <v>1087.75</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2091,46 +2144,96 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>0</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>0</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>40.340000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>6.21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
         <v>0</v>
       </c>
     </row>
@@ -2151,32 +2254,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -2186,27 +2289,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E664DC-F977-477B-8749-D085F1B3AB60}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -2226,20 +2334,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1304F73-03BC-4795-8F16-486EE43DC492}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>